<commit_message>
perbaikan fitur import pengguna
</commit_message>
<xml_diff>
--- a/assets/template_import_pengguna.xlsx
+++ b/assets/template_import_pengguna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\pmb_admin\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ws\htdocs\pmb_admin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE26E926-F25E-4348-A395-DCBDCA2C4DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353D2D4C-9017-4867-88B7-F98CFA4F9AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Nama Pengguna</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Level</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -396,18 +390,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="7" width="11.5703125" hidden="1"/>
+    <col min="8" max="8" width="15.42578125" hidden="1"/>
+    <col min="9" max="16384" width="11.5703125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -428,21 +425,312 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2"/>
+    <row r="17" x14ac:dyDescent="0.2"/>
+    <row r="18" x14ac:dyDescent="0.2"/>
+    <row r="19" x14ac:dyDescent="0.2"/>
+    <row r="20" x14ac:dyDescent="0.2"/>
+    <row r="21" x14ac:dyDescent="0.2"/>
+    <row r="22" x14ac:dyDescent="0.2"/>
+    <row r="23" x14ac:dyDescent="0.2"/>
+    <row r="24" x14ac:dyDescent="0.2"/>
+    <row r="25" x14ac:dyDescent="0.2"/>
+    <row r="26" x14ac:dyDescent="0.2"/>
+    <row r="27" x14ac:dyDescent="0.2"/>
+    <row r="28" x14ac:dyDescent="0.2"/>
+    <row r="29" x14ac:dyDescent="0.2"/>
+    <row r="30" x14ac:dyDescent="0.2"/>
+    <row r="31" x14ac:dyDescent="0.2"/>
+    <row r="32" x14ac:dyDescent="0.2"/>
+    <row r="33" x14ac:dyDescent="0.2"/>
+    <row r="34" x14ac:dyDescent="0.2"/>
+    <row r="35" x14ac:dyDescent="0.2"/>
+    <row r="36" x14ac:dyDescent="0.2"/>
+    <row r="37" x14ac:dyDescent="0.2"/>
+    <row r="38" x14ac:dyDescent="0.2"/>
+    <row r="39" x14ac:dyDescent="0.2"/>
+    <row r="40" x14ac:dyDescent="0.2"/>
+    <row r="41" x14ac:dyDescent="0.2"/>
+    <row r="42" x14ac:dyDescent="0.2"/>
+    <row r="43" x14ac:dyDescent="0.2"/>
+    <row r="44" x14ac:dyDescent="0.2"/>
+    <row r="45" x14ac:dyDescent="0.2"/>
+    <row r="46" x14ac:dyDescent="0.2"/>
+    <row r="47" x14ac:dyDescent="0.2"/>
+    <row r="48" x14ac:dyDescent="0.2"/>
+    <row r="49" x14ac:dyDescent="0.2"/>
+    <row r="50" x14ac:dyDescent="0.2"/>
+    <row r="51" x14ac:dyDescent="0.2"/>
+    <row r="52" x14ac:dyDescent="0.2"/>
+    <row r="53" x14ac:dyDescent="0.2"/>
+    <row r="54" x14ac:dyDescent="0.2"/>
+    <row r="55" x14ac:dyDescent="0.2"/>
+    <row r="56" x14ac:dyDescent="0.2"/>
+    <row r="57" x14ac:dyDescent="0.2"/>
+    <row r="58" x14ac:dyDescent="0.2"/>
+    <row r="59" x14ac:dyDescent="0.2"/>
+    <row r="60" x14ac:dyDescent="0.2"/>
+    <row r="61" x14ac:dyDescent="0.2"/>
+    <row r="62" x14ac:dyDescent="0.2"/>
+    <row r="63" x14ac:dyDescent="0.2"/>
+    <row r="64" x14ac:dyDescent="0.2"/>
+    <row r="65" x14ac:dyDescent="0.2"/>
+    <row r="66" x14ac:dyDescent="0.2"/>
+    <row r="67" x14ac:dyDescent="0.2"/>
+    <row r="68" x14ac:dyDescent="0.2"/>
+    <row r="69" x14ac:dyDescent="0.2"/>
+    <row r="70" x14ac:dyDescent="0.2"/>
+    <row r="71" x14ac:dyDescent="0.2"/>
+    <row r="72" x14ac:dyDescent="0.2"/>
+    <row r="73" x14ac:dyDescent="0.2"/>
+    <row r="74" x14ac:dyDescent="0.2"/>
+    <row r="75" x14ac:dyDescent="0.2"/>
+    <row r="76" x14ac:dyDescent="0.2"/>
+    <row r="77" x14ac:dyDescent="0.2"/>
+    <row r="78" x14ac:dyDescent="0.2"/>
+    <row r="79" x14ac:dyDescent="0.2"/>
+    <row r="80" x14ac:dyDescent="0.2"/>
+    <row r="81" x14ac:dyDescent="0.2"/>
+    <row r="82" x14ac:dyDescent="0.2"/>
+    <row r="83" x14ac:dyDescent="0.2"/>
+    <row r="84" x14ac:dyDescent="0.2"/>
+    <row r="85" x14ac:dyDescent="0.2"/>
+    <row r="86" x14ac:dyDescent="0.2"/>
+    <row r="87" x14ac:dyDescent="0.2"/>
+    <row r="88" x14ac:dyDescent="0.2"/>
+    <row r="89" x14ac:dyDescent="0.2"/>
+    <row r="90" x14ac:dyDescent="0.2"/>
+    <row r="91" x14ac:dyDescent="0.2"/>
+    <row r="92" x14ac:dyDescent="0.2"/>
+    <row r="93" x14ac:dyDescent="0.2"/>
+    <row r="94" x14ac:dyDescent="0.2"/>
+    <row r="95" x14ac:dyDescent="0.2"/>
+    <row r="96" x14ac:dyDescent="0.2"/>
+    <row r="97" x14ac:dyDescent="0.2"/>
+    <row r="98" x14ac:dyDescent="0.2"/>
+    <row r="99" x14ac:dyDescent="0.2"/>
+    <row r="100" x14ac:dyDescent="0.2"/>
+    <row r="101" x14ac:dyDescent="0.2"/>
+    <row r="102" x14ac:dyDescent="0.2"/>
+    <row r="103" x14ac:dyDescent="0.2"/>
+    <row r="104" x14ac:dyDescent="0.2"/>
+    <row r="105" x14ac:dyDescent="0.2"/>
+    <row r="106" x14ac:dyDescent="0.2"/>
+    <row r="107" x14ac:dyDescent="0.2"/>
+    <row r="108" x14ac:dyDescent="0.2"/>
+    <row r="109" x14ac:dyDescent="0.2"/>
+    <row r="110" x14ac:dyDescent="0.2"/>
+    <row r="111" x14ac:dyDescent="0.2"/>
+    <row r="112" x14ac:dyDescent="0.2"/>
+    <row r="113" x14ac:dyDescent="0.2"/>
+    <row r="114" x14ac:dyDescent="0.2"/>
+    <row r="115" x14ac:dyDescent="0.2"/>
+    <row r="116" x14ac:dyDescent="0.2"/>
+    <row r="117" x14ac:dyDescent="0.2"/>
+    <row r="118" x14ac:dyDescent="0.2"/>
+    <row r="119" x14ac:dyDescent="0.2"/>
+    <row r="120" x14ac:dyDescent="0.2"/>
+    <row r="121" x14ac:dyDescent="0.2"/>
+    <row r="122" x14ac:dyDescent="0.2"/>
+    <row r="123" x14ac:dyDescent="0.2"/>
+    <row r="124" x14ac:dyDescent="0.2"/>
+    <row r="125" x14ac:dyDescent="0.2"/>
+    <row r="126" x14ac:dyDescent="0.2"/>
+    <row r="127" x14ac:dyDescent="0.2"/>
+    <row r="128" x14ac:dyDescent="0.2"/>
+    <row r="129" x14ac:dyDescent="0.2"/>
+    <row r="130" x14ac:dyDescent="0.2"/>
+    <row r="131" x14ac:dyDescent="0.2"/>
+    <row r="132" x14ac:dyDescent="0.2"/>
+    <row r="133" x14ac:dyDescent="0.2"/>
+    <row r="134" x14ac:dyDescent="0.2"/>
+    <row r="135" x14ac:dyDescent="0.2"/>
+    <row r="136" x14ac:dyDescent="0.2"/>
+    <row r="137" x14ac:dyDescent="0.2"/>
+    <row r="138" x14ac:dyDescent="0.2"/>
+    <row r="139" x14ac:dyDescent="0.2"/>
+    <row r="140" x14ac:dyDescent="0.2"/>
+    <row r="141" x14ac:dyDescent="0.2"/>
+    <row r="142" x14ac:dyDescent="0.2"/>
+    <row r="143" x14ac:dyDescent="0.2"/>
+    <row r="144" x14ac:dyDescent="0.2"/>
+    <row r="145" x14ac:dyDescent="0.2"/>
+    <row r="146" x14ac:dyDescent="0.2"/>
+    <row r="147" x14ac:dyDescent="0.2"/>
+    <row r="148" x14ac:dyDescent="0.2"/>
+    <row r="149" x14ac:dyDescent="0.2"/>
+    <row r="150" x14ac:dyDescent="0.2"/>
+    <row r="151" x14ac:dyDescent="0.2"/>
+    <row r="152" x14ac:dyDescent="0.2"/>
+    <row r="153" x14ac:dyDescent="0.2"/>
+    <row r="154" x14ac:dyDescent="0.2"/>
+    <row r="155" x14ac:dyDescent="0.2"/>
+    <row r="156" x14ac:dyDescent="0.2"/>
+    <row r="157" x14ac:dyDescent="0.2"/>
+    <row r="158" x14ac:dyDescent="0.2"/>
+    <row r="159" x14ac:dyDescent="0.2"/>
+    <row r="160" x14ac:dyDescent="0.2"/>
+    <row r="161" x14ac:dyDescent="0.2"/>
+    <row r="162" x14ac:dyDescent="0.2"/>
+    <row r="163" x14ac:dyDescent="0.2"/>
+    <row r="164" x14ac:dyDescent="0.2"/>
+    <row r="165" x14ac:dyDescent="0.2"/>
+    <row r="166" x14ac:dyDescent="0.2"/>
+    <row r="167" x14ac:dyDescent="0.2"/>
+    <row r="168" x14ac:dyDescent="0.2"/>
+    <row r="169" x14ac:dyDescent="0.2"/>
+    <row r="170" x14ac:dyDescent="0.2"/>
+    <row r="171" x14ac:dyDescent="0.2"/>
+    <row r="172" x14ac:dyDescent="0.2"/>
+    <row r="173" x14ac:dyDescent="0.2"/>
+    <row r="174" x14ac:dyDescent="0.2"/>
+    <row r="175" x14ac:dyDescent="0.2"/>
+    <row r="176" x14ac:dyDescent="0.2"/>
+    <row r="177" x14ac:dyDescent="0.2"/>
+    <row r="178" x14ac:dyDescent="0.2"/>
+    <row r="179" x14ac:dyDescent="0.2"/>
+    <row r="180" x14ac:dyDescent="0.2"/>
+    <row r="181" x14ac:dyDescent="0.2"/>
+    <row r="182" x14ac:dyDescent="0.2"/>
+    <row r="183" x14ac:dyDescent="0.2"/>
+    <row r="184" x14ac:dyDescent="0.2"/>
+    <row r="185" x14ac:dyDescent="0.2"/>
+    <row r="186" x14ac:dyDescent="0.2"/>
+    <row r="187" x14ac:dyDescent="0.2"/>
+    <row r="188" x14ac:dyDescent="0.2"/>
+    <row r="189" x14ac:dyDescent="0.2"/>
+    <row r="190" x14ac:dyDescent="0.2"/>
+    <row r="191" x14ac:dyDescent="0.2"/>
+    <row r="192" x14ac:dyDescent="0.2"/>
+    <row r="193" x14ac:dyDescent="0.2"/>
+    <row r="194" x14ac:dyDescent="0.2"/>
+    <row r="195" x14ac:dyDescent="0.2"/>
+    <row r="196" x14ac:dyDescent="0.2"/>
+    <row r="197" x14ac:dyDescent="0.2"/>
+    <row r="198" x14ac:dyDescent="0.2"/>
+    <row r="199" x14ac:dyDescent="0.2"/>
+    <row r="200" x14ac:dyDescent="0.2"/>
+    <row r="201" x14ac:dyDescent="0.2"/>
+    <row r="202" x14ac:dyDescent="0.2"/>
+    <row r="203" x14ac:dyDescent="0.2"/>
+    <row r="204" x14ac:dyDescent="0.2"/>
+    <row r="205" x14ac:dyDescent="0.2"/>
+    <row r="206" x14ac:dyDescent="0.2"/>
+    <row r="207" x14ac:dyDescent="0.2"/>
+    <row r="208" x14ac:dyDescent="0.2"/>
+    <row r="209" x14ac:dyDescent="0.2"/>
+    <row r="210" x14ac:dyDescent="0.2"/>
+    <row r="211" x14ac:dyDescent="0.2"/>
+    <row r="212" x14ac:dyDescent="0.2"/>
+    <row r="213" x14ac:dyDescent="0.2"/>
+    <row r="214" x14ac:dyDescent="0.2"/>
+    <row r="215" x14ac:dyDescent="0.2"/>
+    <row r="216" x14ac:dyDescent="0.2"/>
+    <row r="217" x14ac:dyDescent="0.2"/>
+    <row r="218" x14ac:dyDescent="0.2"/>
+    <row r="219" x14ac:dyDescent="0.2"/>
+    <row r="220" x14ac:dyDescent="0.2"/>
+    <row r="221" x14ac:dyDescent="0.2"/>
+    <row r="222" x14ac:dyDescent="0.2"/>
+    <row r="223" x14ac:dyDescent="0.2"/>
+    <row r="224" x14ac:dyDescent="0.2"/>
+    <row r="225" x14ac:dyDescent="0.2"/>
+    <row r="226" x14ac:dyDescent="0.2"/>
+    <row r="227" x14ac:dyDescent="0.2"/>
+    <row r="228" x14ac:dyDescent="0.2"/>
+    <row r="229" x14ac:dyDescent="0.2"/>
+    <row r="230" x14ac:dyDescent="0.2"/>
+    <row r="231" x14ac:dyDescent="0.2"/>
+    <row r="232" x14ac:dyDescent="0.2"/>
+    <row r="233" x14ac:dyDescent="0.2"/>
+    <row r="234" x14ac:dyDescent="0.2"/>
+    <row r="235" x14ac:dyDescent="0.2"/>
+    <row r="236" x14ac:dyDescent="0.2"/>
+    <row r="237" x14ac:dyDescent="0.2"/>
+    <row r="238" x14ac:dyDescent="0.2"/>
+    <row r="239" x14ac:dyDescent="0.2"/>
+    <row r="240" x14ac:dyDescent="0.2"/>
+    <row r="241" x14ac:dyDescent="0.2"/>
+    <row r="242" x14ac:dyDescent="0.2"/>
+    <row r="243" x14ac:dyDescent="0.2"/>
+    <row r="244" x14ac:dyDescent="0.2"/>
+    <row r="245" x14ac:dyDescent="0.2"/>
+    <row r="246" x14ac:dyDescent="0.2"/>
+    <row r="247" x14ac:dyDescent="0.2"/>
+    <row r="248" x14ac:dyDescent="0.2"/>
+    <row r="249" x14ac:dyDescent="0.2"/>
+    <row r="250" x14ac:dyDescent="0.2"/>
+    <row r="251" x14ac:dyDescent="0.2"/>
+    <row r="252" x14ac:dyDescent="0.2"/>
+    <row r="253" x14ac:dyDescent="0.2"/>
+    <row r="254" x14ac:dyDescent="0.2"/>
+    <row r="255" x14ac:dyDescent="0.2"/>
+    <row r="256" x14ac:dyDescent="0.2"/>
+    <row r="257" x14ac:dyDescent="0.2"/>
+    <row r="258" x14ac:dyDescent="0.2"/>
+    <row r="259" x14ac:dyDescent="0.2"/>
+    <row r="260" x14ac:dyDescent="0.2"/>
+    <row r="261" x14ac:dyDescent="0.2"/>
+    <row r="262" x14ac:dyDescent="0.2"/>
+    <row r="263" x14ac:dyDescent="0.2"/>
+    <row r="264" x14ac:dyDescent="0.2"/>
+    <row r="265" x14ac:dyDescent="0.2"/>
+    <row r="266" x14ac:dyDescent="0.2"/>
+    <row r="267" x14ac:dyDescent="0.2"/>
+    <row r="268" x14ac:dyDescent="0.2"/>
+    <row r="269" x14ac:dyDescent="0.2"/>
+    <row r="270" x14ac:dyDescent="0.2"/>
+    <row r="271" x14ac:dyDescent="0.2"/>
+    <row r="272" x14ac:dyDescent="0.2"/>
+    <row r="273" x14ac:dyDescent="0.2"/>
+    <row r="274" x14ac:dyDescent="0.2"/>
+    <row r="275" x14ac:dyDescent="0.2"/>
+    <row r="276" x14ac:dyDescent="0.2"/>
+    <row r="277" x14ac:dyDescent="0.2"/>
+    <row r="278" x14ac:dyDescent="0.2"/>
+    <row r="279" x14ac:dyDescent="0.2"/>
+    <row r="280" x14ac:dyDescent="0.2"/>
+    <row r="281" x14ac:dyDescent="0.2"/>
+    <row r="282" x14ac:dyDescent="0.2"/>
+    <row r="283" x14ac:dyDescent="0.2"/>
+    <row r="284" x14ac:dyDescent="0.2"/>
+    <row r="285" x14ac:dyDescent="0.2"/>
+    <row r="286" x14ac:dyDescent="0.2"/>
+    <row r="287" x14ac:dyDescent="0.2"/>
+    <row r="288" x14ac:dyDescent="0.2"/>
+    <row r="289" x14ac:dyDescent="0.2"/>
+    <row r="290" x14ac:dyDescent="0.2"/>
+    <row r="291" x14ac:dyDescent="0.2"/>
+    <row r="292" x14ac:dyDescent="0.2"/>
+    <row r="293" x14ac:dyDescent="0.2"/>
+    <row r="294" x14ac:dyDescent="0.2"/>
+    <row r="295" x14ac:dyDescent="0.2"/>
+    <row r="296" x14ac:dyDescent="0.2"/>
+    <row r="297" x14ac:dyDescent="0.2"/>
+    <row r="298" x14ac:dyDescent="0.2"/>
+    <row r="299" x14ac:dyDescent="0.2"/>
+    <row r="300" x14ac:dyDescent="0.2"/>
+    <row r="301" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D301" xr:uid="{9CC3C717-870F-4CDD-92D1-0F746CEC3351}">
+      <formula1>"admin,guru"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>